<commit_message>
UCAC hip stars reading
</commit_message>
<xml_diff>
--- a/SpPh.xlsx
+++ b/SpPh.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr showObjects="none" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHubStorage\Astrometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="2400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="2400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BV" sheetId="1" r:id="rId1"/>
     <sheet name="Teff" sheetId="2" r:id="rId2"/>
+    <sheet name="Sp" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>F0</t>
   </si>
@@ -85,6 +86,15 @@
   </si>
   <si>
     <t>SpType</t>
+  </si>
+  <si>
+    <t>G0</t>
+  </si>
+  <si>
+    <t>K0</t>
+  </si>
+  <si>
+    <t>M5</t>
   </si>
 </sst>
 </file>
@@ -406,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -617,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,10 +660,10 @@
         <v>6500</v>
       </c>
       <c r="B3">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="C3">
-        <v>2.9</v>
+        <v>6540</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -663,8 +673,11 @@
       <c r="A4">
         <v>6250</v>
       </c>
+      <c r="B4">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="C4">
-        <v>4.5</v>
+        <v>5925</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,7 +688,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C5">
-        <v>6.3</v>
+        <v>5564</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -686,7 +699,7 @@
         <v>5750</v>
       </c>
       <c r="C6">
-        <v>7.8</v>
+        <v>5122</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -700,7 +713,7 @@
         <v>0.71</v>
       </c>
       <c r="C7">
-        <v>8.1999999999999993</v>
+        <v>4456</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -711,7 +724,7 @@
         <v>5250</v>
       </c>
       <c r="C8">
-        <v>8.1999999999999993</v>
+        <v>4011</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,7 +735,7 @@
         <v>0.9</v>
       </c>
       <c r="C9">
-        <v>7.7</v>
+        <v>3870</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -772,4 +785,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.3</v>
+      </c>
+      <c r="C2">
+        <v>7078</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.42</v>
+      </c>
+      <c r="C3">
+        <v>6540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C4">
+        <v>5925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.69</v>
+      </c>
+      <c r="C5">
+        <v>5564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>0.85</v>
+      </c>
+      <c r="C6">
+        <v>5122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C7">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1.42</v>
+      </c>
+      <c r="C8">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>1.61</v>
+      </c>
+      <c r="C9">
+        <v>3870</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>